<commit_message>
Fix Package email batch detection: add delay after batch marker creation to prevent race condition
</commit_message>
<xml_diff>
--- a/WB_Test_Report_2025-12-24.xlsx
+++ b/WB_Test_Report_2025-12-24.xlsx
@@ -435,7 +435,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="str">
-        <v>BOP (OH)</v>
+        <v>BOP (WI)</v>
       </c>
       <c r="C2" t="str">
         <v>N/A</v>
@@ -447,10 +447,10 @@
         <v>FAILED</v>
       </c>
       <c r="F2" t="str">
-        <v>272.89</v>
+        <v>222.81</v>
       </c>
       <c r="G2" t="str">
-        <v>OH</v>
+        <v>WI</v>
       </c>
     </row>
     <row r="3">
@@ -458,22 +458,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="str">
-        <v>BOP (WI)</v>
+        <v>BOP (DE)</v>
       </c>
       <c r="C3" t="str">
-        <v>3002611343</v>
+        <v>3003179622</v>
       </c>
       <c r="D3" t="str">
-        <v>1002229282</v>
+        <v>1003052773</v>
       </c>
       <c r="E3" t="str">
         <v>PASSED</v>
       </c>
       <c r="F3" t="str">
-        <v>443.36</v>
+        <v>464.79</v>
       </c>
       <c r="G3" t="str">
-        <v>WI</v>
+        <v>DE</v>
       </c>
     </row>
     <row r="4">
@@ -481,22 +481,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="str">
-        <v>BOP (PA)</v>
+        <v>BOP (WI)</v>
       </c>
       <c r="C4" t="str">
-        <v>3002611344</v>
+        <v>3003179624</v>
       </c>
       <c r="D4" t="str">
-        <v>1002229283</v>
+        <v>1003052774</v>
       </c>
       <c r="E4" t="str">
         <v>PASSED</v>
       </c>
       <c r="F4" t="str">
-        <v>449.74</v>
+        <v>486.61</v>
       </c>
       <c r="G4" t="str">
-        <v>PA</v>
+        <v>WI</v>
       </c>
     </row>
     <row r="5">
@@ -507,16 +507,16 @@
         <v>BOP (MI)</v>
       </c>
       <c r="C5" t="str">
-        <v>3002611348</v>
+        <v>N/A</v>
       </c>
       <c r="D5" t="str">
-        <v>1002229284</v>
+        <v>N/A</v>
       </c>
       <c r="E5" t="str">
-        <v>PASSED</v>
+        <v>FAILED</v>
       </c>
       <c r="F5" t="str">
-        <v>474.60</v>
+        <v>107.42</v>
       </c>
       <c r="G5" t="str">
         <v>MI</v>
@@ -527,22 +527,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="str">
-        <v>BOP (DE)</v>
+        <v>BOP (OH)</v>
       </c>
       <c r="C6" t="str">
-        <v>3002611347</v>
+        <v>3003179627</v>
       </c>
       <c r="D6" t="str">
-        <v>1002229285</v>
+        <v>1003052775</v>
       </c>
       <c r="E6" t="str">
         <v>PASSED</v>
       </c>
       <c r="F6" t="str">
-        <v>503.92</v>
+        <v>455.67</v>
       </c>
       <c r="G6" t="str">
-        <v>DE</v>
+        <v>OH</v>
       </c>
     </row>
   </sheetData>
@@ -554,7 +554,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -581,10 +581,10 @@
         <v>PASSED</v>
       </c>
       <c r="C2" t="str">
-        <v>70.59s</v>
+        <v>68.82s</v>
       </c>
       <c r="D2" t="str">
-        <v>2025-12-24T18:02:33.333Z</v>
+        <v>2025-12-24T18:53:11.574Z</v>
       </c>
     </row>
     <row r="3">
@@ -595,29 +595,15 @@
         <v>PASSED</v>
       </c>
       <c r="C3" t="str">
-        <v>136.43s</v>
+        <v>153.99s</v>
       </c>
       <c r="D3" t="str">
-        <v>2025-12-24T18:04:49.760Z</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Test Execution Failed</v>
-      </c>
-      <c r="B4" t="str">
-        <v>FAILED</v>
-      </c>
-      <c r="C4" t="str">
-        <v>65.87s</v>
-      </c>
-      <c r="D4" t="str">
-        <v>2025-12-24T18:05:55.633Z</v>
+        <v>2025-12-24T18:55:45.570Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -651,10 +637,10 @@
         <v>PASSED</v>
       </c>
       <c r="C2" t="str">
-        <v>71.53s</v>
+        <v>72.13s</v>
       </c>
       <c r="D2" t="str">
-        <v>2025-12-24T18:02:33.726Z</v>
+        <v>2025-12-24T18:53:11.104Z</v>
       </c>
     </row>
     <row r="3">
@@ -665,10 +651,10 @@
         <v>PASSED</v>
       </c>
       <c r="C3" t="str">
-        <v>132.56s</v>
+        <v>135.97s</v>
       </c>
       <c r="D3" t="str">
-        <v>2025-12-24T18:04:46.285Z</v>
+        <v>2025-12-24T18:55:27.079Z</v>
       </c>
     </row>
     <row r="4">
@@ -679,10 +665,10 @@
         <v>PASSED</v>
       </c>
       <c r="C4" t="str">
-        <v>20.42s</v>
+        <v>22.91s</v>
       </c>
       <c r="D4" t="str">
-        <v>2025-12-24T18:05:06.711Z</v>
+        <v>2025-12-24T18:55:49.996Z</v>
       </c>
     </row>
     <row r="5">
@@ -693,10 +679,10 @@
         <v>PASSED</v>
       </c>
       <c r="C5" t="str">
-        <v>32.54s</v>
+        <v>34.73s</v>
       </c>
       <c r="D5" t="str">
-        <v>2025-12-24T18:05:39.258Z</v>
+        <v>2025-12-24T18:56:24.724Z</v>
       </c>
     </row>
     <row r="6">
@@ -707,10 +693,10 @@
         <v>PASSED</v>
       </c>
       <c r="C6" t="str">
-        <v>40.27s</v>
+        <v>50.86s</v>
       </c>
       <c r="D6" t="str">
-        <v>2025-12-24T18:06:19.526Z</v>
+        <v>2025-12-24T18:57:15.581Z</v>
       </c>
     </row>
     <row r="7">
@@ -721,10 +707,10 @@
         <v>PASSED</v>
       </c>
       <c r="C7" t="str">
-        <v>146.04s</v>
+        <v>148.19s</v>
       </c>
       <c r="D7" t="str">
-        <v>2025-12-24T18:08:45.566Z</v>
+        <v>2025-12-24T18:59:43.776Z</v>
       </c>
     </row>
   </sheetData>
@@ -763,10 +749,10 @@
         <v>PASSED</v>
       </c>
       <c r="C2" t="str">
-        <v>70.72s</v>
+        <v>68.82s</v>
       </c>
       <c r="D2" t="str">
-        <v>2025-12-24T18:02:38.852Z</v>
+        <v>2025-12-24T18:53:11.574Z</v>
       </c>
     </row>
     <row r="3">
@@ -777,10 +763,10 @@
         <v>PASSED</v>
       </c>
       <c r="C3" t="str">
-        <v>131.03s</v>
+        <v>153.99s</v>
       </c>
       <c r="D3" t="str">
-        <v>2025-12-24T18:04:49.882Z</v>
+        <v>2025-12-24T18:55:45.570Z</v>
       </c>
     </row>
     <row r="4">
@@ -791,10 +777,10 @@
         <v>PASSED</v>
       </c>
       <c r="C4" t="str">
-        <v>31.51s</v>
+        <v>33.64s</v>
       </c>
       <c r="D4" t="str">
-        <v>2025-12-24T18:05:21.391Z</v>
+        <v>2025-12-24T18:56:19.215Z</v>
       </c>
     </row>
     <row r="5">
@@ -805,10 +791,10 @@
         <v>PASSED</v>
       </c>
       <c r="C5" t="str">
-        <v>30.97s</v>
+        <v>35.54s</v>
       </c>
       <c r="D5" t="str">
-        <v>2025-12-24T18:05:52.364Z</v>
+        <v>2025-12-24T18:56:54.758Z</v>
       </c>
     </row>
     <row r="6">
@@ -819,10 +805,10 @@
         <v>PASSED</v>
       </c>
       <c r="C6" t="str">
-        <v>40.76s</v>
+        <v>44.05s</v>
       </c>
       <c r="D6" t="str">
-        <v>2025-12-24T18:06:33.125Z</v>
+        <v>2025-12-24T18:57:38.809Z</v>
       </c>
     </row>
     <row r="7">
@@ -833,10 +819,10 @@
         <v>PASSED</v>
       </c>
       <c r="C7" t="str">
-        <v>144.75s</v>
+        <v>150.57s</v>
       </c>
       <c r="D7" t="str">
-        <v>2025-12-24T18:08:57.881Z</v>
+        <v>2025-12-24T19:00:09.381Z</v>
       </c>
     </row>
   </sheetData>
@@ -848,7 +834,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -869,91 +855,21 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Account Created</v>
+        <v>Test Execution Failed</v>
       </c>
       <c r="B2" t="str">
-        <v>PASSED</v>
+        <v>FAILED</v>
       </c>
       <c r="C2" t="str">
-        <v>69.85s</v>
+        <v>107.42s</v>
       </c>
       <c r="D2" t="str">
-        <v>2025-12-24T18:10:13.319Z</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Building and Classification Added</v>
-      </c>
-      <c r="B3" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C3" t="str">
-        <v>137.06s</v>
-      </c>
-      <c r="D3" t="str">
-        <v>2025-12-24T18:12:30.380Z</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Quote Rated Successfully</v>
-      </c>
-      <c r="B4" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C4" t="str">
-        <v>26.58s</v>
-      </c>
-      <c r="D4" t="str">
-        <v>2025-12-24T18:12:56.962Z</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Submitting for Approval</v>
-      </c>
-      <c r="B5" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C5" t="str">
-        <v>49.42s</v>
-      </c>
-      <c r="D5" t="str">
-        <v>2025-12-24T18:13:46.385Z</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>UW Issues Approved in PolicyCenter</v>
-      </c>
-      <c r="B6" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C6" t="str">
-        <v>46.13s</v>
-      </c>
-      <c r="D6" t="str">
-        <v>2025-12-24T18:14:32.516Z</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>Policy Issued Successfully</v>
-      </c>
-      <c r="B7" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C7" t="str">
-        <v>145.56s</v>
-      </c>
-      <c r="D7" t="str">
-        <v>2025-12-24T18:16:58.079Z</v>
+        <v>2025-12-24T19:02:02.109Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -987,10 +903,10 @@
         <v>PASSED</v>
       </c>
       <c r="C2" t="str">
-        <v>70.25s</v>
+        <v>69.80s</v>
       </c>
       <c r="D2" t="str">
-        <v>2025-12-24T18:10:13.569Z</v>
+        <v>2025-12-24T19:01:24.529Z</v>
       </c>
     </row>
     <row r="3">
@@ -1001,10 +917,10 @@
         <v>PASSED</v>
       </c>
       <c r="C3" t="str">
-        <v>138.08s</v>
+        <v>133.29s</v>
       </c>
       <c r="D3" t="str">
-        <v>2025-12-24T18:12:31.654Z</v>
+        <v>2025-12-24T19:03:37.820Z</v>
       </c>
     </row>
     <row r="4">
@@ -1015,10 +931,10 @@
         <v>PASSED</v>
       </c>
       <c r="C4" t="str">
-        <v>27.53s</v>
+        <v>27.18s</v>
       </c>
       <c r="D4" t="str">
-        <v>2025-12-24T18:12:59.182Z</v>
+        <v>2025-12-24T19:04:04.998Z</v>
       </c>
     </row>
     <row r="5">
@@ -1029,10 +945,10 @@
         <v>PASSED</v>
       </c>
       <c r="C5" t="str">
-        <v>71.55s</v>
+        <v>35.69s</v>
       </c>
       <c r="D5" t="str">
-        <v>2025-12-24T18:14:10.732Z</v>
+        <v>2025-12-24T19:04:40.689Z</v>
       </c>
     </row>
     <row r="6">
@@ -1043,10 +959,10 @@
         <v>PASSED</v>
       </c>
       <c r="C6" t="str">
-        <v>50.32s</v>
+        <v>41.07s</v>
       </c>
       <c r="D6" t="str">
-        <v>2025-12-24T18:15:01.051Z</v>
+        <v>2025-12-24T19:05:21.762Z</v>
       </c>
     </row>
     <row r="7">
@@ -1057,10 +973,10 @@
         <v>PASSED</v>
       </c>
       <c r="C7" t="str">
-        <v>146.19s</v>
+        <v>148.64s</v>
       </c>
       <c r="D7" t="str">
-        <v>2025-12-24T18:17:27.247Z</v>
+        <v>2025-12-24T19:07:50.402Z</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Runners: flexible args; don't require env first; include first token as state when env omitted
</commit_message>
<xml_diff>
--- a/WB_Test_Report_2025-12-24.xlsx
+++ b/WB_Test_Report_2025-12-24.xlsx
@@ -4,11 +4,8 @@
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
-    <sheet name="BOP_1" sheetId="2" r:id="rId2"/>
-    <sheet name="BOP_2" sheetId="3" r:id="rId3"/>
-    <sheet name="BOP_3" sheetId="4" r:id="rId4"/>
-    <sheet name="BOP_4" sheetId="5" r:id="rId5"/>
-    <sheet name="BOP_5" sheetId="6" r:id="rId6"/>
+    <sheet name="Package_1" sheetId="2" r:id="rId2"/>
+    <sheet name="Package_2" sheetId="3" r:id="rId3"/>
   </sheets>
 </workbook>
 </file>
@@ -402,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -435,7 +432,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="str">
-        <v>BOP (WI)</v>
+        <v>Package (PA)</v>
       </c>
       <c r="C2" t="str">
         <v>N/A</v>
@@ -447,10 +444,10 @@
         <v>FAILED</v>
       </c>
       <c r="F2" t="str">
-        <v>222.81</v>
+        <v>141.13</v>
       </c>
       <c r="G2" t="str">
-        <v>WI</v>
+        <v>PA</v>
       </c>
     </row>
     <row r="3">
@@ -458,96 +455,27 @@
         <v>2</v>
       </c>
       <c r="B3" t="str">
-        <v>BOP (DE)</v>
+        <v>Package (MI)</v>
       </c>
       <c r="C3" t="str">
-        <v>3003179622</v>
+        <v>3003179637</v>
       </c>
       <c r="D3" t="str">
-        <v>1003052773</v>
+        <v>N/A</v>
       </c>
       <c r="E3" t="str">
-        <v>PASSED</v>
+        <v>FAILED</v>
       </c>
       <c r="F3" t="str">
-        <v>464.79</v>
+        <v>154.31</v>
       </c>
       <c r="G3" t="str">
-        <v>DE</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="str">
-        <v>BOP (WI)</v>
-      </c>
-      <c r="C4" t="str">
-        <v>3003179624</v>
-      </c>
-      <c r="D4" t="str">
-        <v>1003052774</v>
-      </c>
-      <c r="E4" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="F4" t="str">
-        <v>486.61</v>
-      </c>
-      <c r="G4" t="str">
-        <v>WI</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="str">
-        <v>BOP (MI)</v>
-      </c>
-      <c r="C5" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="D5" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="E5" t="str">
-        <v>FAILED</v>
-      </c>
-      <c r="F5" t="str">
-        <v>107.42</v>
-      </c>
-      <c r="G5" t="str">
         <v>MI</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="str">
-        <v>BOP (OH)</v>
-      </c>
-      <c r="C6" t="str">
-        <v>3003179627</v>
-      </c>
-      <c r="D6" t="str">
-        <v>1003052775</v>
-      </c>
-      <c r="E6" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="F6" t="str">
-        <v>455.67</v>
-      </c>
-      <c r="G6" t="str">
-        <v>OH</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G3"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -581,24 +509,24 @@
         <v>PASSED</v>
       </c>
       <c r="C2" t="str">
-        <v>68.82s</v>
+        <v>75.09s</v>
       </c>
       <c r="D2" t="str">
-        <v>2025-12-24T18:53:11.574Z</v>
+        <v>2025-12-24T23:47:15.105Z</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Building and Classification Added</v>
+        <v>Test Execution Failed</v>
       </c>
       <c r="B3" t="str">
-        <v>PASSED</v>
+        <v>FAILED</v>
       </c>
       <c r="C3" t="str">
-        <v>153.99s</v>
+        <v>66.04s</v>
       </c>
       <c r="D3" t="str">
-        <v>2025-12-24T18:55:45.570Z</v>
+        <v>2025-12-24T23:48:21.150Z</v>
       </c>
     </row>
   </sheetData>
@@ -610,7 +538,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -637,351 +565,29 @@
         <v>PASSED</v>
       </c>
       <c r="C2" t="str">
-        <v>72.13s</v>
+        <v>75.15s</v>
       </c>
       <c r="D2" t="str">
-        <v>2025-12-24T18:53:11.104Z</v>
+        <v>2025-12-24T23:47:15.368Z</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Building and Classification Added</v>
+        <v>Test Execution Failed</v>
       </c>
       <c r="B3" t="str">
-        <v>PASSED</v>
+        <v>FAILED</v>
       </c>
       <c r="C3" t="str">
-        <v>135.97s</v>
+        <v>79.16s</v>
       </c>
       <c r="D3" t="str">
-        <v>2025-12-24T18:55:27.079Z</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Quote Rated Successfully</v>
-      </c>
-      <c r="B4" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C4" t="str">
-        <v>22.91s</v>
-      </c>
-      <c r="D4" t="str">
-        <v>2025-12-24T18:55:49.996Z</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Submitting for Approval</v>
-      </c>
-      <c r="B5" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C5" t="str">
-        <v>34.73s</v>
-      </c>
-      <c r="D5" t="str">
-        <v>2025-12-24T18:56:24.724Z</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>UW Issues Approved in PolicyCenter</v>
-      </c>
-      <c r="B6" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C6" t="str">
-        <v>50.86s</v>
-      </c>
-      <c r="D6" t="str">
-        <v>2025-12-24T18:57:15.581Z</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>Policy Issued Successfully</v>
-      </c>
-      <c r="B7" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C7" t="str">
-        <v>148.19s</v>
-      </c>
-      <c r="D7" t="str">
-        <v>2025-12-24T18:59:43.776Z</v>
+        <v>2025-12-24T23:48:34.529Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D7"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Milestone</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Status</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Duration (s)</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Timestamp</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Account Created</v>
-      </c>
-      <c r="B2" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C2" t="str">
-        <v>68.82s</v>
-      </c>
-      <c r="D2" t="str">
-        <v>2025-12-24T18:53:11.574Z</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Building and Classification Added</v>
-      </c>
-      <c r="B3" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C3" t="str">
-        <v>153.99s</v>
-      </c>
-      <c r="D3" t="str">
-        <v>2025-12-24T18:55:45.570Z</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Quote Rated Successfully</v>
-      </c>
-      <c r="B4" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C4" t="str">
-        <v>33.64s</v>
-      </c>
-      <c r="D4" t="str">
-        <v>2025-12-24T18:56:19.215Z</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Submitting for Approval</v>
-      </c>
-      <c r="B5" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C5" t="str">
-        <v>35.54s</v>
-      </c>
-      <c r="D5" t="str">
-        <v>2025-12-24T18:56:54.758Z</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>UW Issues Approved in PolicyCenter</v>
-      </c>
-      <c r="B6" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C6" t="str">
-        <v>44.05s</v>
-      </c>
-      <c r="D6" t="str">
-        <v>2025-12-24T18:57:38.809Z</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>Policy Issued Successfully</v>
-      </c>
-      <c r="B7" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C7" t="str">
-        <v>150.57s</v>
-      </c>
-      <c r="D7" t="str">
-        <v>2025-12-24T19:00:09.381Z</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D7"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Milestone</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Status</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Duration (s)</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Timestamp</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Test Execution Failed</v>
-      </c>
-      <c r="B2" t="str">
-        <v>FAILED</v>
-      </c>
-      <c r="C2" t="str">
-        <v>107.42s</v>
-      </c>
-      <c r="D2" t="str">
-        <v>2025-12-24T19:02:02.109Z</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Milestone</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Status</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Duration (s)</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Timestamp</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Account Created</v>
-      </c>
-      <c r="B2" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C2" t="str">
-        <v>69.80s</v>
-      </c>
-      <c r="D2" t="str">
-        <v>2025-12-24T19:01:24.529Z</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Building and Classification Added</v>
-      </c>
-      <c r="B3" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C3" t="str">
-        <v>133.29s</v>
-      </c>
-      <c r="D3" t="str">
-        <v>2025-12-24T19:03:37.820Z</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Quote Rated Successfully</v>
-      </c>
-      <c r="B4" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C4" t="str">
-        <v>27.18s</v>
-      </c>
-      <c r="D4" t="str">
-        <v>2025-12-24T19:04:04.998Z</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Submitting for Approval</v>
-      </c>
-      <c r="B5" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C5" t="str">
-        <v>35.69s</v>
-      </c>
-      <c r="D5" t="str">
-        <v>2025-12-24T19:04:40.689Z</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>UW Issues Approved in PolicyCenter</v>
-      </c>
-      <c r="B6" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C6" t="str">
-        <v>41.07s</v>
-      </c>
-      <c r="D6" t="str">
-        <v>2025-12-24T19:05:21.762Z</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>Policy Issued Successfully</v>
-      </c>
-      <c r="B7" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C7" t="str">
-        <v>148.64s</v>
-      </c>
-      <c r="D7" t="str">
-        <v>2025-12-24T19:07:50.402Z</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>